<commit_message>
More IR calibration, Std deviation, etc
</commit_message>
<xml_diff>
--- a/IRDistanceCalibration.xlsx
+++ b/IRDistanceCalibration.xlsx
@@ -175,22 +175,22 @@
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>280</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>265</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>185</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>178</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>170</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -262,11 +262,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="88306048"/>
-        <c:axId val="88307584"/>
+        <c:axId val="86143360"/>
+        <c:axId val="86144896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88306048"/>
+        <c:axId val="86143360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -276,12 +276,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88307584"/>
+        <c:crossAx val="86144896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88307584"/>
+        <c:axId val="86144896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -292,7 +292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88306048"/>
+        <c:crossAx val="86143360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -318,16 +318,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -639,7 +639,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,12 +685,12 @@
         <v>32</v>
       </c>
       <c r="I2">
-        <f>(E7-E2)/(D7-D2)</f>
-        <v>-2.2727272727272728E-2</v>
+        <f>(E3-E2)/(D3-D2)</f>
+        <v>-1.8181818181818181E-2</v>
       </c>
       <c r="K2">
         <f>INT(I2*100000)</f>
-        <v>-2273</v>
+        <v>-1819</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -701,12 +701,12 @@
         <v>11</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I16" si="0">(E8-E3)/(D8-D3)</f>
-        <v>-2.553191489361702E-2</v>
+        <f t="shared" ref="I3:I16" si="0">(E4-E3)/(D4-D3)</f>
+        <v>-2.0408163265306121E-2</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K16" si="1">INT(I3*100000)</f>
-        <v>-2554</v>
+        <v>-2041</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -718,11 +718,11 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>-3.0303030303030304E-2</v>
+        <v>-2.7777777777777776E-2</v>
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
-        <v>-3031</v>
+        <v>-2778</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -734,11 +734,11 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>-4.2105263157894736E-2</v>
+        <v>-2.2727272727272728E-2</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>-4211</v>
+        <v>-2273</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -750,11 +750,11 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>-5.2287581699346407E-2</v>
+        <v>-2.7777777777777776E-2</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>-5229</v>
+        <v>-2778</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -776,11 +776,11 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>-6.8965517241379309E-2</v>
+        <v>-2.8571428571428571E-2</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>-6897</v>
+        <v>-2858</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -792,11 +792,11 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>-9.7872340425531917E-2</v>
+        <v>-3.8461538461538464E-2</v>
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>-9788</v>
+        <v>-3847</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -818,11 +818,11 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>-0.11792452830188679</v>
+        <v>-8.771929824561403E-2</v>
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>-11793</v>
+        <v>-8772</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -834,11 +834,11 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>-0.1388888888888889</v>
+        <v>-7.6923076923076927E-2</v>
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>-13889</v>
+        <v>-7693</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -860,27 +860,27 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>-0.20491803278688525</v>
+        <v>-0.14285714285714285</v>
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>-20492</v>
+        <v>-14286</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="E12">
         <v>35</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>-0.22727272727272727</v>
+        <v>-0.17857142857142858</v>
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>-22728</v>
+        <v>-17858</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -891,22 +891,22 @@
         <v>50</v>
       </c>
       <c r="D13">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="E13">
         <v>40</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0.15094339622641509</v>
+        <v>-0.18518518518518517</v>
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>15094</v>
+        <v>-18519</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -918,11 +918,11 @@
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>0.21428571428571427</v>
+        <v>-0.18518518518518517</v>
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>21428</v>
+        <v>-18519</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -933,7 +933,7 @@
         <v>70</v>
       </c>
       <c r="D15">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E15">
         <v>50</v>
@@ -944,11 +944,11 @@
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>0.27027027027027029</v>
+        <v>-0.38461538461538464</v>
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>27027</v>
+        <v>-38462</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -959,22 +959,22 @@
         <v>80</v>
       </c>
       <c r="D16">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E16">
         <v>55</v>
       </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>0.3089887640449438</v>
+        <v>-0.25</v>
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>30898</v>
+        <v>-25000</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -985,14 +985,14 @@
         <v>90</v>
       </c>
       <c r="D17">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="E17">
         <v>60</v>
       </c>
       <c r="G17">
         <f t="shared" si="2"/>
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>